<commit_message>
Correct PDO sensitivity descriptions in Lecture 02 materials for clarity
</commit_message>
<xml_diff>
--- a/score_PDO_example.xlsx
+++ b/score_PDO_example.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiuw\Dropbox\_Teaching\Northwestern MLDS\Interpretable ML for Finance\IML4Finance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\_Teaching\Northwestern MLDS\Interpretable ML for Finance\IML4Finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6C238A1-F18C-43E9-B69E-106485A2CA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A81C9A-F6D8-42E6-B0B6-064B1ACF12EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8295" yWindow="3750" windowWidth="14730" windowHeight="10875" xr2:uid="{1EF45B99-6CE3-405B-86EF-D83C6BF2EBF3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" activeTab="1" xr2:uid="{1EF45B99-6CE3-405B-86EF-D83C6BF2EBF3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Example1" sheetId="1" r:id="rId1"/>
+    <sheet name="Example2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>A</t>
   </si>
@@ -69,6 +70,18 @@
   </si>
   <si>
     <t>n</t>
+  </si>
+  <si>
+    <t>PDO</t>
+  </si>
+  <si>
+    <t>Score_PDO20</t>
+  </si>
+  <si>
+    <t>Score_PDO40</t>
+  </si>
+  <si>
+    <t>delta</t>
   </si>
 </sst>
 </file>
@@ -443,13 +456,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9AFF8CA-78C9-4944-B80F-46276C727EE8}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +470,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -466,7 +479,7 @@
         <v>28.85390081777927</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -498,7 +511,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.01</v>
       </c>
@@ -530,7 +543,7 @@
         <v>1.0101010101010102E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.02</v>
       </c>
@@ -562,7 +575,7 @@
         <v>20</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I6:I18" si="4">G6-H6</f>
+        <f t="shared" ref="I6:I17" si="4">G6-H6</f>
         <v>980</v>
       </c>
       <c r="J6">
@@ -570,7 +583,7 @@
         <v>2.0408163265306121E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.03</v>
       </c>
@@ -610,7 +623,7 @@
         <v>3.0927835051546393E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.04</v>
       </c>
@@ -650,7 +663,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.05</v>
       </c>
@@ -690,7 +703,7 @@
         <v>5.2631578947368418E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.06</v>
       </c>
@@ -730,7 +743,7 @@
         <v>6.3829787234042548E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -770,7 +783,7 @@
         <v>7.5268817204301078E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.08</v>
       </c>
@@ -810,7 +823,7 @@
         <v>8.6956521739130432E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.09</v>
       </c>
@@ -850,7 +863,7 @@
         <v>9.8901098901098897E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.1</v>
       </c>
@@ -890,7 +903,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.15</v>
       </c>
@@ -930,7 +943,7 @@
         <v>0.17647058823529413</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.2</v>
       </c>
@@ -970,7 +983,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.25</v>
       </c>
@@ -1008,6 +1021,231 @@
       <c r="J17">
         <f t="shared" si="5"/>
         <v>0.33333333333333331</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCD02EB-AE93-4FF9-B8BB-591FE960235F}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1">
+        <v>20</v>
+      </c>
+      <c r="E1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>600</v>
+      </c>
+      <c r="E2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f>D1/LN(2)</f>
+        <v>28.85390081777927</v>
+      </c>
+      <c r="E3">
+        <f>E1/LN(2)</f>
+        <v>57.707801635558539</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>0.01</v>
+      </c>
+      <c r="B6">
+        <f>A6/(1-A6)</f>
+        <v>1.0101010101010102E-2</v>
+      </c>
+      <c r="C6">
+        <f>LN(B6)</f>
+        <v>-4.5951198501345898</v>
+      </c>
+      <c r="D6" s="1">
+        <f>D$2-D$3*$C6</f>
+        <v>732.58713240159216</v>
+      </c>
+      <c r="E6" s="1">
+        <f>E$2-E$3*$C6</f>
+        <v>865.17426480318431</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>0.02</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ref="B7:B10" si="0">A7/(1-A7)</f>
+        <v>2.0408163265306124E-2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:C10" si="1">LN(B7)</f>
+        <v>-3.8918202981106265</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" ref="D7:E10" si="2">D$2-D$3*$C7</f>
+        <v>712.29419688230416</v>
+      </c>
+      <c r="E7" s="1">
+        <f t="shared" si="2"/>
+        <v>824.58839376460833</v>
+      </c>
+      <c r="G7" s="1">
+        <f>D7-D6</f>
+        <v>-20.292935519287994</v>
+      </c>
+      <c r="H7" s="1">
+        <f>E7-E6</f>
+        <v>-40.585871038575988</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>0.03</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>3.0927835051546393E-2</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>-3.4760986898352733</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="2"/>
+        <v>700.29900682931941</v>
+      </c>
+      <c r="E8" s="1">
+        <f t="shared" si="2"/>
+        <v>800.59801365863882</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" ref="G8:G10" si="3">D8-D7</f>
+        <v>-11.995190052984753</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" ref="H8:H10" si="4">E8-E7</f>
+        <v>-23.990380105969507</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>0.04</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666671E-2</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>-3.1780538303479453</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="2"/>
+        <v>691.69925001442311</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="2"/>
+        <v>783.39850002884623</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="3"/>
+        <v>-8.5997568148962955</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="4"/>
+        <v>-17.199513629792591</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>0.05</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>5.2631578947368425E-2</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>-2.9444389791664403</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="2"/>
+        <v>684.9585502688717</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" si="2"/>
+        <v>769.91710053774341</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="3"/>
+        <v>-6.7406997455514102</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="4"/>
+        <v>-13.48139949110282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
draft of Lab 02.qmd
</commit_message>
<xml_diff>
--- a/score_PDO_example.xlsx
+++ b/score_PDO_example.xlsx
@@ -1,21 +1,49 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Dropbox\_Teaching\Northwestern MLDS\Interpretable ML for Finance\IML4Finance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamchiu/Dropbox/_Teaching/Northwestern MLDS/Interpretable ML for Finance/IML4Finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A81C9A-F6D8-42E6-B0B6-064B1ACF12EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E836501-1055-0E4E-9F44-C15E2315708C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" activeTab="1" xr2:uid="{1EF45B99-6CE3-405B-86EF-D83C6BF2EBF3}"/>
+    <workbookView xWindow="5700" yWindow="1880" windowWidth="29920" windowHeight="17000" activeTab="1" xr2:uid="{1EF45B99-6CE3-405B-86EF-D83C6BF2EBF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Example1" sheetId="1" r:id="rId1"/>
     <sheet name="Example2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">Example2!$D$2</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_lin" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Example2!$F$8</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -88,7 +116,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0000000000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,15 +154,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -460,9 +505,9 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +515,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -479,7 +524,7 @@
         <v>28.85390081777927</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -511,7 +556,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>0.01</v>
       </c>
@@ -543,7 +588,7 @@
         <v>1.0101010101010102E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.02</v>
       </c>
@@ -583,7 +628,7 @@
         <v>2.0408163265306121E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>0.03</v>
       </c>
@@ -623,7 +668,7 @@
         <v>3.0927835051546393E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0.04</v>
       </c>
@@ -663,7 +708,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>0.05</v>
       </c>
@@ -703,7 +748,7 @@
         <v>5.2631578947368418E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>0.06</v>
       </c>
@@ -743,7 +788,7 @@
         <v>6.3829787234042548E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -783,7 +828,7 @@
         <v>7.5268817204301078E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>0.08</v>
       </c>
@@ -823,7 +868,7 @@
         <v>8.6956521739130432E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>0.09</v>
       </c>
@@ -863,7 +908,7 @@
         <v>9.8901098901098897E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.1</v>
       </c>
@@ -903,7 +948,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.15</v>
       </c>
@@ -943,7 +988,7 @@
         <v>0.17647058823529413</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.2</v>
       </c>
@@ -983,7 +1028,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.25</v>
       </c>
@@ -1030,22 +1075,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BCD02EB-AE93-4FF9-B8BB-591FE960235F}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
         <v>11</v>
       </c>
@@ -1056,18 +1102,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>600</v>
+        <v>650.29900682931941</v>
       </c>
       <c r="E2">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>1</v>
       </c>
@@ -1080,7 +1126,7 @@
         <v>57.707801635558539</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G4" t="s">
         <v>14</v>
       </c>
@@ -1088,7 +1134,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1111,46 +1157,46 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
         <v>0.01</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="3">
         <f>A6/(1-A6)</f>
         <v>1.0101010101010102E-2</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <f>LN(B6)</f>
         <v>-4.5951198501345898</v>
       </c>
       <c r="D6" s="1">
         <f>D$2-D$3*$C6</f>
-        <v>732.58713240159216</v>
+        <v>782.88613923091157</v>
       </c>
       <c r="E6" s="1">
         <f>E$2-E$3*$C6</f>
-        <v>865.17426480318431</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7">
+        <v>815.17426480318431</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
         <v>0.02</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <f t="shared" ref="B7:B10" si="0">A7/(1-A7)</f>
         <v>2.0408163265306124E-2</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <f t="shared" ref="C7:C10" si="1">LN(B7)</f>
         <v>-3.8918202981106265</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" ref="D7:E10" si="2">D$2-D$3*$C7</f>
-        <v>712.29419688230416</v>
+        <v>762.59320371162357</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="2"/>
-        <v>824.58839376460833</v>
+        <v>774.58839376460833</v>
       </c>
       <c r="G7" s="1">
         <f>D7-D6</f>
@@ -1161,26 +1207,27 @@
         <v>-40.585871038575988</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
         <v>0.03</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <f t="shared" si="0"/>
         <v>3.0927835051546393E-2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <f t="shared" si="1"/>
         <v>-3.4760986898352733</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="2"/>
-        <v>700.29900682931941</v>
+        <v>750.59801365863882</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="2"/>
-        <v>800.59801365863882</v>
-      </c>
+        <v>750.59801365863882</v>
+      </c>
+      <c r="F8" s="4"/>
       <c r="G8" s="1">
         <f t="shared" ref="G8:G10" si="3">D8-D7</f>
         <v>-11.995190052984753</v>
@@ -1190,25 +1237,25 @@
         <v>-23.990380105969507</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
         <v>0.04</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <f t="shared" si="0"/>
         <v>4.1666666666666671E-2</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <f t="shared" si="1"/>
         <v>-3.1780538303479453</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="2"/>
-        <v>691.69925001442311</v>
+        <v>741.99825684374252</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="2"/>
-        <v>783.39850002884623</v>
+        <v>733.39850002884623</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="3"/>
@@ -1219,25 +1266,25 @@
         <v>-17.199513629792591</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
         <v>0.05</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <f t="shared" si="0"/>
         <v>5.2631578947368425E-2</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <f t="shared" si="1"/>
         <v>-2.9444389791664403</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="2"/>
-        <v>684.9585502688717</v>
+        <v>735.25755709819111</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="2"/>
-        <v>769.91710053774341</v>
+        <v>719.91710053774341</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="3"/>
@@ -1246,6 +1293,12 @@
       <c r="H10" s="1">
         <f t="shared" si="4"/>
         <v>-13.48139949110282</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="3">
+        <f>1/B6</f>
+        <v>98.999999999999986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>